<commit_message>
Changed to correct values.
</commit_message>
<xml_diff>
--- a/pos20_2_cycle1.xlsx
+++ b/pos20_2_cycle1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olle de Jong\Documents\Github\ProteinTranslocationModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A163C4-5F50-4152-968A-245CC3EC4960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07353A45-1BD9-49FB-8A07-1B8E14E92A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1875" yWindow="3240" windowWidth="16290" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -434,13 +434,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>41.914423708681227</v>
+        <v>41.883597547754363</v>
       </c>
       <c r="C3">
-        <v>16.90890820191601</v>
+        <v>17.036402832147122</v>
       </c>
       <c r="D3">
-        <v>6.4739535168642517</v>
+        <v>6.5429032225398212</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -448,13 +448,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>42.025397888017949</v>
+        <v>41.963745566164206</v>
       </c>
       <c r="C4">
-        <v>16.449927533083979</v>
+        <v>16.704916793546221</v>
       </c>
       <c r="D4">
-        <v>6.2257345764321999</v>
+        <v>6.3636339877833388</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -462,13 +462,13 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>42.136372067354678</v>
+        <v>42.043893584574072</v>
       </c>
       <c r="C5">
-        <v>15.99094686425196</v>
+        <v>16.373430754945311</v>
       </c>
       <c r="D5">
-        <v>5.9775156360001471</v>
+        <v>6.1843647530268573</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -476,13 +476,13 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>42.247346246691407</v>
+        <v>42.12404160298393</v>
       </c>
       <c r="C6">
-        <v>15.53196619541994</v>
+        <v>16.0419447163444</v>
       </c>
       <c r="D6">
-        <v>5.7292966955680944</v>
+        <v>6.0050955182703749</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -490,13 +490,13 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>42.358320426028143</v>
+        <v>42.204189621393787</v>
       </c>
       <c r="C7">
-        <v>15.07298552658791</v>
+        <v>15.7104586777435</v>
       </c>
       <c r="D7">
-        <v>5.4810777551360417</v>
+        <v>5.8258262835138934</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -504,13 +504,13 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>42.634467972952613</v>
+        <v>42.284337639803653</v>
       </c>
       <c r="C8">
-        <v>15.05586543790843</v>
+        <v>15.37897263914259</v>
       </c>
       <c r="D8">
-        <v>5.4782157010536929</v>
+        <v>5.6465570487574102</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -518,13 +518,13 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>43.075788887464832</v>
+        <v>42.364485658213511</v>
       </c>
       <c r="C9">
-        <v>15.4806059293815</v>
+        <v>15.04748660054168</v>
       </c>
       <c r="D9">
-        <v>5.7207105333210464</v>
+        <v>5.4672878140009278</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -532,13 +532,13 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>43.517109801977057</v>
+        <v>42.53639665861656</v>
       </c>
       <c r="C10">
-        <v>15.90534642085456</v>
+        <v>14.961478662025529</v>
       </c>
       <c r="D10">
-        <v>5.9632053655884008</v>
+        <v>5.424327960549836</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -546,13 +546,13 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>43.958430716489282</v>
+        <v>42.855128430208723</v>
       </c>
       <c r="C11">
-        <v>16.330086912327619</v>
+        <v>15.26823568364496</v>
       </c>
       <c r="D11">
-        <v>6.2057001978557542</v>
+        <v>5.5994631171873701</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -560,13 +560,13 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>44.399751631001507</v>
+        <v>43.173860201800878</v>
       </c>
       <c r="C12">
-        <v>16.754827403800689</v>
+        <v>15.5749927052644</v>
       </c>
       <c r="D12">
-        <v>6.4481950301231086</v>
+        <v>5.7745982738249033</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -574,13 +574,13 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>44.841072545513732</v>
+        <v>43.49259197339304</v>
       </c>
       <c r="C13">
-        <v>17.179567895273749</v>
+        <v>15.881749726883831</v>
       </c>
       <c r="D13">
-        <v>6.6906898623904629</v>
+        <v>5.9497334304624374</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -588,13 +588,13 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>45.057649183745923</v>
+        <v>43.811323744985202</v>
       </c>
       <c r="C14">
-        <v>17.067086798878009</v>
+        <v>16.188506748503269</v>
       </c>
       <c r="D14">
-        <v>6.6255136472488054</v>
+        <v>6.1248685870999697</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -602,13 +602,13 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>45.274225821978121</v>
+        <v>44.130055516577357</v>
       </c>
       <c r="C15">
-        <v>16.954605702482262</v>
+        <v>16.495263770122701</v>
       </c>
       <c r="D15">
-        <v>6.5603374321071488</v>
+        <v>6.3000037437375038</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -616,13 +616,13 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>45.490802460210311</v>
+        <v>44.448787288169527</v>
       </c>
       <c r="C16">
-        <v>16.842124606086511</v>
+        <v>16.802020791742141</v>
       </c>
       <c r="D16">
-        <v>6.4951612169654913</v>
+        <v>6.475138900375037</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -630,13 +630,13 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>45.707379098442502</v>
+        <v>44.767519059761689</v>
       </c>
       <c r="C17">
-        <v>16.729643509690771</v>
+        <v>17.10877781336157</v>
       </c>
       <c r="D17">
-        <v>6.4299850018238338</v>
+        <v>6.6502740570125702</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -644,13 +644,13 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>45.923955736674692</v>
+        <v>44.961392900087169</v>
       </c>
       <c r="C18">
-        <v>16.61716241329502</v>
+        <v>17.117078397276121</v>
       </c>
       <c r="D18">
-        <v>6.3648087866821772</v>
+        <v>6.6544808539784306</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -658,13 +658,13 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>45.998844093439601</v>
+        <v>45.117809361032641</v>
       </c>
       <c r="C19">
-        <v>16.762529923831199</v>
+        <v>17.035842049879189</v>
       </c>
       <c r="D19">
-        <v>6.4514798789872856</v>
+        <v>6.6074091430427897</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -672,13 +672,13 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>45.932044168737207</v>
+        <v>45.274225821978114</v>
       </c>
       <c r="C20">
-        <v>17.1657460412993</v>
+        <v>16.954605702482262</v>
       </c>
       <c r="D20">
-        <v>6.6899982787391634</v>
+        <v>6.5603374321071488</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -686,13 +686,13 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>45.865244244034827</v>
+        <v>45.430642282923593</v>
       </c>
       <c r="C21">
-        <v>17.568962158767398</v>
+        <v>16.87336935508533</v>
       </c>
       <c r="D21">
-        <v>6.9285166784910386</v>
+        <v>6.513265721171507</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -700,13 +700,13 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>45.798444319332447</v>
+        <v>45.587058743869058</v>
       </c>
       <c r="C22">
-        <v>17.9721782762355</v>
+        <v>16.79213300768841</v>
       </c>
       <c r="D22">
-        <v>7.1670350782429164</v>
+        <v>6.4661940102358653</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -714,13 +714,13 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>45.731644394630067</v>
+        <v>45.74347520481453</v>
       </c>
       <c r="C23">
-        <v>18.375394393703601</v>
+        <v>16.710896660291478</v>
       </c>
       <c r="D23">
-        <v>7.4055534779947934</v>
+        <v>6.4191222993002244</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -728,13 +728,13 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>45.664844469927679</v>
+        <v>45.899891665760009</v>
       </c>
       <c r="C24">
-        <v>18.778610511171699</v>
+        <v>16.629660312894551</v>
       </c>
       <c r="D24">
-        <v>7.6440718777466703</v>
+        <v>6.3720505883645826</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -742,13 +742,13 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>45.722985258411427</v>
+        <v>46.024821841934973</v>
       </c>
       <c r="C25">
-        <v>19.03137347666463</v>
+        <v>16.605723655926941</v>
       </c>
       <c r="D25">
-        <v>7.802051649153154</v>
+        <v>6.3587227235282233</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -756,13 +756,13 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>45.781126046895167</v>
+        <v>45.976577451872139</v>
       </c>
       <c r="C26">
-        <v>19.284136442157561</v>
+        <v>16.896935296320571</v>
       </c>
       <c r="D26">
-        <v>7.9600314205596394</v>
+        <v>6.5309860122379124</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -770,13 +770,13 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>45.839266835378908</v>
+        <v>45.928333061809298</v>
       </c>
       <c r="C27">
-        <v>19.53689940765048</v>
+        <v>17.18814693671419</v>
       </c>
       <c r="D27">
-        <v>8.1180111919661222</v>
+        <v>6.7032493009476006</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -784,13 +784,13 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>45.897407623862662</v>
+        <v>45.880088671746471</v>
       </c>
       <c r="C28">
-        <v>19.789662373143411</v>
+        <v>17.479358577107821</v>
       </c>
       <c r="D28">
-        <v>8.2759909633726068</v>
+        <v>6.8755125896572888</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -798,13 +798,13 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>45.95554841234641</v>
+        <v>45.831844281683637</v>
       </c>
       <c r="C29">
-        <v>20.042425338636349</v>
+        <v>17.770570217501451</v>
       </c>
       <c r="D29">
-        <v>8.4339707347790913</v>
+        <v>7.0477758783669779</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -812,13 +812,13 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>45.971209263458192</v>
+        <v>45.78359989162081</v>
       </c>
       <c r="C30">
-        <v>20.007985218438161</v>
+        <v>18.061781857895081</v>
       </c>
       <c r="D30">
-        <v>8.4118399781281123</v>
+        <v>7.220039167076667</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -826,13 +826,13 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>45.944390177198002</v>
+        <v>45.735355501557983</v>
       </c>
       <c r="C31">
-        <v>19.686342012548849</v>
+        <v>18.352993498288701</v>
       </c>
       <c r="D31">
-        <v>8.2095986934196699</v>
+        <v>7.3923024557863561</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -840,13 +840,13 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>45.917571090937813</v>
+        <v>45.687111111495142</v>
       </c>
       <c r="C32">
-        <v>19.36469880665955</v>
+        <v>18.644205138682331</v>
       </c>
       <c r="D32">
-        <v>8.0073574087112274</v>
+        <v>7.5645657444960452</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -854,13 +854,13 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>45.890752004677623</v>
+        <v>45.687454776560237</v>
       </c>
       <c r="C33">
-        <v>19.043055600770241</v>
+        <v>18.876907219974498</v>
       </c>
       <c r="D33">
-        <v>7.8051161240027831</v>
+        <v>7.7055084555158588</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -868,13 +868,13 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>45.86393291841744</v>
+        <v>45.729445346020732</v>
       </c>
       <c r="C34">
-        <v>18.721412394880939</v>
+        <v>19.05945825060828</v>
       </c>
       <c r="D34">
-        <v>7.6028748392943406</v>
+        <v>7.8196049570872086</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -882,13 +882,13 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>45.83711383215725</v>
+        <v>45.771435915481213</v>
       </c>
       <c r="C35">
-        <v>18.39976918899163</v>
+        <v>19.242009281242069</v>
       </c>
       <c r="D35">
-        <v>7.4006335545858972</v>
+        <v>7.9337014586585566</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -896,13 +896,13 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>46.17321555264148</v>
+        <v>45.813426484941687</v>
       </c>
       <c r="C36">
-        <v>18.536618623778558</v>
+        <v>19.424560311875851</v>
       </c>
       <c r="D36">
-        <v>7.4876610832330046</v>
+        <v>8.0477979602299072</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -910,13 +910,13 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>46.50931727312571</v>
+        <v>45.855417054402182</v>
       </c>
       <c r="C37">
-        <v>18.67346805856549</v>
+        <v>19.607111342509629</v>
       </c>
       <c r="D37">
-        <v>7.5746886118801138</v>
+        <v>8.161894461801257</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -924,13 +924,13 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>46.84541899360994</v>
+        <v>45.897407623862662</v>
       </c>
       <c r="C38">
-        <v>18.810317493352422</v>
+        <v>19.789662373143411</v>
       </c>
       <c r="D38">
-        <v>7.6617161405272221</v>
+        <v>8.2759909633726068</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -938,13 +938,13 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>47.181520714094169</v>
+        <v>45.939398193323143</v>
       </c>
       <c r="C39">
-        <v>18.94716692813935</v>
+        <v>19.9722134037772</v>
       </c>
       <c r="D39">
-        <v>7.7487436691743303</v>
+        <v>8.3900874649439565</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -952,13 +952,13 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>47.517622434578399</v>
+        <v>45.981388762783631</v>
       </c>
       <c r="C40">
-        <v>19.08401636292627</v>
+        <v>20.154764434410978</v>
       </c>
       <c r="D40">
-        <v>7.8357711978214386</v>
+        <v>8.5041839665153063</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -966,13 +966,13 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>47.774518906773643</v>
+        <v>45.966739415748158</v>
       </c>
       <c r="C41">
-        <v>19.217538515410109</v>
+        <v>19.954378017456609</v>
       </c>
       <c r="D41">
-        <v>7.916451330392726</v>
+        <v>8.3781330973433707</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -980,13 +980,13 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>47.952210130679887</v>
+        <v>45.947370075671351</v>
       </c>
       <c r="C42">
-        <v>19.34773338559085</v>
+        <v>19.722080146536548</v>
       </c>
       <c r="D42">
-        <v>7.9907840668881924</v>
+        <v>8.2320699472761625</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -994,13 +994,13 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>48.129901354586153</v>
+        <v>45.928000735594551</v>
       </c>
       <c r="C43">
-        <v>19.477928255771591</v>
+        <v>19.489782275616498</v>
       </c>
       <c r="D43">
-        <v>8.0651168033836562</v>
+        <v>8.0860067972089542</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1008,13 +1008,13 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>48.307592578492397</v>
+        <v>45.908631395517752</v>
       </c>
       <c r="C44">
-        <v>19.608123125952329</v>
+        <v>19.257484404696442</v>
       </c>
       <c r="D44">
-        <v>8.1394495398791218</v>
+        <v>7.9399436471417442</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1022,13 +1022,13 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>48.485283802398662</v>
+        <v>45.889262055440938</v>
       </c>
       <c r="C45">
-        <v>19.73831799613307</v>
+        <v>19.025186533776392</v>
       </c>
       <c r="D45">
-        <v>8.2137822763745856</v>
+        <v>7.7938804970745359</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1036,13 +1036,13 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>48.662975026304913</v>
+        <v>45.869892715364138</v>
       </c>
       <c r="C46">
-        <v>19.868512866313811</v>
+        <v>18.792888662856331</v>
       </c>
       <c r="D46">
-        <v>8.2881150128700511</v>
+        <v>7.6478173470073267</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1050,13 +1050,13 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>48.82426979988265</v>
+        <v>45.850523375287352</v>
       </c>
       <c r="C47">
-        <v>19.896293122933201</v>
+        <v>18.560590791936281</v>
       </c>
       <c r="D47">
-        <v>8.3019150780361333</v>
+        <v>7.5017541969401176</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1064,13 +1064,13 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>48.985564573460387</v>
+        <v>45.911803103375973</v>
       </c>
       <c r="C48">
-        <v>19.924073379552599</v>
+        <v>18.430180174499839</v>
       </c>
       <c r="D48">
-        <v>8.3157151432022154</v>
+        <v>7.4199730053963648</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1078,13 +1078,13 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>49.146859347038131</v>
+        <v>46.154543234836801</v>
       </c>
       <c r="C49">
-        <v>19.95185363617199</v>
+        <v>18.529015877401509</v>
       </c>
       <c r="D49">
-        <v>8.3295152083682993</v>
+        <v>7.4828262205303879</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1092,13 +1092,13 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>49.308154120615868</v>
+        <v>46.397283366297643</v>
       </c>
       <c r="C50">
-        <v>19.97963389279138</v>
+        <v>18.627851580303179</v>
       </c>
       <c r="D50">
-        <v>8.3433152735343814</v>
+        <v>7.5456794356644101</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1106,13 +1106,13 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>49.469448894193619</v>
+        <v>46.64002349775847</v>
       </c>
       <c r="C51">
-        <v>20.007414149410771</v>
+        <v>18.72668728320485</v>
       </c>
       <c r="D51">
-        <v>8.3571153387004635</v>
+        <v>7.6085326507984332</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1120,13 +1120,13 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>49.699068091528879</v>
+        <v>46.882763629219298</v>
       </c>
       <c r="C52">
-        <v>20.04491616776221</v>
+        <v>18.82552298610652</v>
       </c>
       <c r="D52">
-        <v>8.3767616257060471</v>
+        <v>7.6713858659324563</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1134,13 +1134,13 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>49.997011712621671</v>
+        <v>47.125503760680139</v>
       </c>
       <c r="C53">
-        <v>20.09213994784567</v>
+        <v>18.924358689008191</v>
       </c>
       <c r="D53">
-        <v>8.4022541345511321</v>
+        <v>7.7342390810664794</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1148,13 +1148,13 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>50.294955333714462</v>
+        <v>47.368243892140967</v>
       </c>
       <c r="C54">
-        <v>20.13936372792914</v>
+        <v>19.023194391909861</v>
       </c>
       <c r="D54">
-        <v>8.4277466433962172</v>
+        <v>7.7970922962005016</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1162,13 +1162,13 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>50.592898954807247</v>
+        <v>47.610984023601809</v>
       </c>
       <c r="C55">
-        <v>20.186587508012611</v>
+        <v>19.122030094811539</v>
       </c>
       <c r="D55">
-        <v>8.4532391522413022</v>
+        <v>7.8599455113345256</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1176,13 +1176,13 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>50.890842575900031</v>
+        <v>47.77451890677365</v>
       </c>
       <c r="C56">
-        <v>20.233811288096081</v>
+        <v>19.217538515410109</v>
       </c>
       <c r="D56">
-        <v>8.4787316610863872</v>
+        <v>7.916451330392726</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1190,13 +1190,13 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>51.188786196992822</v>
+        <v>47.902851457372613</v>
       </c>
       <c r="C57">
-        <v>20.281035068179548</v>
+        <v>19.311568143873981</v>
       </c>
       <c r="D57">
-        <v>8.5042241699314722</v>
+        <v>7.97013608452834</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1204,13 +1204,13 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>51.819100639565733</v>
+        <v>48.031184007971568</v>
       </c>
       <c r="C58">
-        <v>20.48772029664504</v>
+        <v>19.405597772337849</v>
       </c>
       <c r="D58">
-        <v>8.6318447880654396</v>
+        <v>8.0238208386639531</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1218,13 +1218,13 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>52.449415082138643</v>
+        <v>48.15951655857053</v>
       </c>
       <c r="C59">
-        <v>20.69440552511054</v>
+        <v>19.499627400801721</v>
       </c>
       <c r="D59">
-        <v>8.7594654061994088</v>
+        <v>8.077505592799568</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1232,13 +1232,13 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>53.079729524711539</v>
+        <v>48.287849109169493</v>
       </c>
       <c r="C60">
-        <v>20.901090753576039</v>
+        <v>19.593657029265589</v>
       </c>
       <c r="D60">
-        <v>8.8870860243333762</v>
+        <v>8.1311903469351812</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1246,13 +1246,13 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>53.710043967284442</v>
+        <v>48.416181659768448</v>
       </c>
       <c r="C61">
-        <v>21.107775982041531</v>
+        <v>19.687686657729451</v>
       </c>
       <c r="D61">
-        <v>9.0147066424673437</v>
+        <v>8.1848751010707943</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1260,13 +1260,13 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>54.340358409857352</v>
+        <v>48.544514210367403</v>
       </c>
       <c r="C62">
-        <v>21.31446121050703</v>
+        <v>19.781716286193319</v>
       </c>
       <c r="D62">
-        <v>9.1423272606013128</v>
+        <v>8.2385598552064074</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1274,13 +1274,13 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>54.844604440331572</v>
+        <v>48.671935847059217</v>
       </c>
       <c r="C63">
-        <v>21.22773658119133</v>
+        <v>19.87005621390378</v>
       </c>
       <c r="D63">
-        <v>9.0667791743363502</v>
+        <v>8.2888816831570562</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1288,13 +1288,13 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>55.222782058707082</v>
+        <v>48.788426516865371</v>
       </c>
       <c r="C64">
-        <v>20.847602094094409</v>
+        <v>19.890119732573339</v>
       </c>
       <c r="D64">
-        <v>8.7880623836724574</v>
+        <v>8.2988483968881148</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1302,13 +1302,13 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>55.600959677082599</v>
+        <v>48.904917186671518</v>
       </c>
       <c r="C65">
-        <v>20.467467606997491</v>
+        <v>19.910183251242898</v>
       </c>
       <c r="D65">
-        <v>8.5093455930085646</v>
+        <v>8.3088151106191752</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1316,13 +1316,13 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>55.979137295458123</v>
+        <v>49.021407856477673</v>
       </c>
       <c r="C66">
-        <v>20.08733311990057</v>
+        <v>19.930246769912461</v>
       </c>
       <c r="D66">
-        <v>8.2306288023446701</v>
+        <v>8.3187818243502356</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1330,13 +1330,13 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>56.357314913833633</v>
+        <v>49.13789852628382</v>
       </c>
       <c r="C67">
-        <v>19.70719863280366</v>
+        <v>19.95031028858202</v>
       </c>
       <c r="D67">
-        <v>7.9519120116807764</v>
+        <v>8.3287485380812942</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1344,13 +1344,13 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>56.73549253220915</v>
+        <v>49.254389196089967</v>
       </c>
       <c r="C68">
-        <v>19.327064145706739</v>
+        <v>19.97037380725159</v>
       </c>
       <c r="D68">
-        <v>7.6731952210168828</v>
+        <v>8.3387152518123546</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1358,13 +1358,13 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>57.23293755822047</v>
+        <v>49.370879865896107</v>
       </c>
       <c r="C69">
-        <v>18.361354555285651</v>
+        <v>19.99043732592115</v>
       </c>
       <c r="D69">
-        <v>7.1601681406770377</v>
+        <v>8.3486819655434132</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1372,13 +1372,13 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>57.730382584231783</v>
+        <v>49.487370535702262</v>
       </c>
       <c r="C70">
-        <v>17.395644964864552</v>
+        <v>20.010500844590709</v>
       </c>
       <c r="D70">
-        <v>6.6471410603371908</v>
+        <v>8.3586486792744736</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1386,13 +1386,13 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>58.227827610243097</v>
+        <v>49.649410821346763</v>
       </c>
       <c r="C71">
-        <v>16.429935374443449</v>
+        <v>20.037045537748291</v>
       </c>
       <c r="D71">
-        <v>6.1341139799973439</v>
+        <v>8.3725128742318677</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1400,13 +1400,13 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>58.72527263625441</v>
+        <v>49.864592325469317</v>
       </c>
       <c r="C72">
-        <v>15.46422578402235</v>
+        <v>20.07115160114191</v>
       </c>
       <c r="D72">
-        <v>5.621086899657497</v>
+        <v>8.3909241306199842</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1414,13 +1414,13 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>59.222717662265723</v>
+        <v>50.079773829591893</v>
       </c>
       <c r="C73">
-        <v>14.498516193601249</v>
+        <v>20.105257664535529</v>
       </c>
       <c r="D73">
-        <v>5.1080598193176554</v>
+        <v>8.4093353870081007</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1428,13 +1428,13 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>58.146504953538077</v>
+        <v>50.294955333714462</v>
       </c>
       <c r="C74">
-        <v>13.84414414072509</v>
+        <v>20.13936372792914</v>
       </c>
       <c r="D74">
-        <v>4.7606041370598096</v>
+        <v>8.4277466433962172</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1442,13 +1442,13 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>55.496634510071402</v>
+        <v>50.510136837837031</v>
       </c>
       <c r="C75">
-        <v>13.501109625393889</v>
+        <v>20.173469791322759</v>
       </c>
       <c r="D75">
-        <v>4.5787198528839763</v>
+        <v>8.4461578997843354</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1456,13 +1456,13 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>52.84676406660472</v>
+        <v>50.7253183419596</v>
       </c>
       <c r="C76">
-        <v>13.158075110062679</v>
+        <v>20.207575854716382</v>
       </c>
       <c r="D76">
-        <v>4.3968355687081422</v>
+        <v>8.4645691561724519</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -1470,13 +1470,13 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>50.196893623138038</v>
+        <v>50.940499846082169</v>
       </c>
       <c r="C77">
-        <v>12.815040594731469</v>
+        <v>20.24168191810999</v>
       </c>
       <c r="D77">
-        <v>4.2149512845323081</v>
+        <v>8.4829804125605683</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1484,13 +1484,13 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>47.547023179671363</v>
+        <v>51.155681350204738</v>
       </c>
       <c r="C78">
-        <v>12.47200607940027</v>
+        <v>20.275787981503608</v>
       </c>
       <c r="D78">
-        <v>4.0330670003564739</v>
+        <v>8.5013916689486848</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1498,13 +1498,13 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>44.897152736204667</v>
+        <v>51.573978356342927</v>
       </c>
       <c r="C79">
-        <v>12.12897156406906</v>
+        <v>20.407342707797358</v>
       </c>
       <c r="D79">
-        <v>3.8511827161806398</v>
+        <v>8.5822145476800085</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1512,13 +1512,13 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>45.260730028591773</v>
+        <v>52.029205453756703</v>
       </c>
       <c r="C80">
-        <v>12.640666728992411</v>
+        <v>20.556615372800209</v>
       </c>
       <c r="D80">
-        <v>4.1311243405699702</v>
+        <v>8.6743849941100972</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1526,13 +1526,13 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>45.624307320978893</v>
+        <v>52.484432551170471</v>
       </c>
       <c r="C81">
-        <v>13.152361893915771</v>
+        <v>20.705888037803071</v>
       </c>
       <c r="D81">
-        <v>4.411065964959306</v>
+        <v>8.7665554405401842</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1540,13 +1540,13 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>45.98788461336602</v>
+        <v>52.939659648584239</v>
       </c>
       <c r="C82">
-        <v>13.66405705883912</v>
+        <v>20.855160702805929</v>
       </c>
       <c r="D82">
-        <v>4.6910075893486409</v>
+        <v>8.858725886970273</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1554,13 +1554,13 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>46.351461905753141</v>
+        <v>53.394886745998001</v>
       </c>
       <c r="C83">
-        <v>14.17575222376248</v>
+        <v>21.00443336780879</v>
       </c>
       <c r="D83">
-        <v>4.9709492137379758</v>
+        <v>8.9508963334003599</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1568,13 +1568,13 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>46.715039198140268</v>
+        <v>53.850113843411769</v>
       </c>
       <c r="C84">
-        <v>14.687447388685831</v>
+        <v>21.153706032811652</v>
       </c>
       <c r="D84">
-        <v>5.2508908381273116</v>
+        <v>9.0430667798304487</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1582,13 +1582,13 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>46.733195185115598</v>
+        <v>54.305340940825538</v>
       </c>
       <c r="C85">
-        <v>14.753397641792811</v>
+        <v>21.30297869781451</v>
       </c>
       <c r="D85">
-        <v>5.2947433389164322</v>
+        <v>9.1352372262605375</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1596,13 +1596,13 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>46.405929866679173</v>
+        <v>54.718545234206402</v>
       </c>
       <c r="C86">
-        <v>14.373602983083421</v>
+        <v>21.354448076890289</v>
       </c>
       <c r="D86">
-        <v>5.102506716105335</v>
+        <v>9.1596847712243132</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1610,13 +1610,13 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>46.078664548242728</v>
+        <v>54.991673514144267</v>
       </c>
       <c r="C87">
-        <v>13.993808324374029</v>
+        <v>21.079906502875851</v>
       </c>
       <c r="D87">
-        <v>4.9102700932942387</v>
+        <v>8.9583893113003903</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -1624,13 +1624,13 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>45.751399229806282</v>
+        <v>55.264801794082153</v>
       </c>
       <c r="C88">
-        <v>13.614013665664629</v>
+        <v>20.805364928861419</v>
       </c>
       <c r="D88">
-        <v>4.7180334704831397</v>
+        <v>8.7570938513764673</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -1638,13 +1638,13 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>45.424133911369843</v>
+        <v>55.537930074020018</v>
       </c>
       <c r="C89">
-        <v>13.234219006955239</v>
+        <v>20.530823354846969</v>
       </c>
       <c r="D89">
-        <v>4.5257968476720443</v>
+        <v>8.5557983914525444</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -1652,13 +1652,13 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>45.096868592933397</v>
+        <v>55.811058353957897</v>
       </c>
       <c r="C90">
-        <v>12.854424348245839</v>
+        <v>20.256281780832531</v>
       </c>
       <c r="D90">
-        <v>4.3335602248609444</v>
+        <v>8.3545029315286197</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -1666,13 +1666,13 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>46.017969583854352</v>
+        <v>56.084186633895769</v>
       </c>
       <c r="C91">
-        <v>13.048797814599849</v>
+        <v>19.981740206818099</v>
       </c>
       <c r="D91">
-        <v>4.4316688664434043</v>
+        <v>8.1532074716046985</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -1680,13 +1680,13 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>46.939070574775293</v>
+        <v>56.35731491383364</v>
       </c>
       <c r="C92">
-        <v>13.24317128095387</v>
+        <v>19.707198632803649</v>
       </c>
       <c r="D92">
-        <v>4.5297775080258642</v>
+        <v>7.9519120116807747</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -1694,13 +1694,13 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>47.860171565696263</v>
+        <v>56.630443193771512</v>
       </c>
       <c r="C93">
-        <v>13.437544747307889</v>
+        <v>19.432657058789211</v>
       </c>
       <c r="D93">
-        <v>4.627886149608325</v>
+        <v>7.7506165517568508</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -1708,13 +1708,13 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>48.781272556617211</v>
+        <v>56.956579210436409</v>
       </c>
       <c r="C94">
-        <v>13.631918213661899</v>
+        <v>18.897859883297361</v>
       </c>
       <c r="D94">
-        <v>4.7259947911907849</v>
+        <v>7.4451831853102819</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -1722,13 +1722,13 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>49.702373547538173</v>
+        <v>57.315845062555688</v>
       </c>
       <c r="C95">
-        <v>13.82629168001592</v>
+        <v>18.20040295688213</v>
       </c>
       <c r="D95">
-        <v>4.8241034327732466</v>
+        <v>7.0746636272870624</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -1736,13 +1736,13 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>49.982333985109427</v>
+        <v>57.675110914674967</v>
       </c>
       <c r="C96">
-        <v>13.936397086432841</v>
+        <v>17.50294603046688</v>
       </c>
       <c r="D96">
-        <v>4.8788401858328836</v>
+        <v>6.7041440692638394</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -1750,13 +1750,13 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>49.621153869330939</v>
+        <v>58.034376766794253</v>
       </c>
       <c r="C97">
-        <v>13.96223443291268</v>
+        <v>16.805489104051649</v>
       </c>
       <c r="D97">
-        <v>4.8902050503696977</v>
+        <v>6.3336245112406147</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -1764,13 +1764,13 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>49.259973753552458</v>
+        <v>58.393642618913518</v>
       </c>
       <c r="C98">
-        <v>13.988071779392509</v>
+        <v>16.10803217763641</v>
       </c>
       <c r="D98">
-        <v>4.90156991490651</v>
+        <v>5.9631049532173952</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -1778,13 +1778,13 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>48.898793637773963</v>
+        <v>58.752908471032811</v>
       </c>
       <c r="C99">
-        <v>14.01390912587234</v>
+        <v>15.41057525122117</v>
       </c>
       <c r="D99">
-        <v>4.9129347794433231</v>
+        <v>5.5925853951941713</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -1792,13 +1792,13 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>48.537613521995482</v>
+        <v>59.11217432315209</v>
       </c>
       <c r="C100">
-        <v>14.039746472352171</v>
+        <v>14.713118324805929</v>
       </c>
       <c r="D100">
-        <v>4.9242996439801354</v>
+        <v>5.2220658371709474</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -1806,13 +1806,13 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>48.176433406216987</v>
+        <v>59.471440175271383</v>
       </c>
       <c r="C101">
-        <v>14.065583818832</v>
+        <v>14.015661398390691</v>
       </c>
       <c r="D101">
-        <v>4.9356645085169486</v>
+        <v>4.8515462791477244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>